<commit_message>
proyecto BI GEOESPACIAL PYTHON
</commit_message>
<xml_diff>
--- a/clientes_con_cobertura.xlsx
+++ b/clientes_con_cobertura.xlsx
@@ -645,23 +645,23 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Av. Salverry 300</t>
+          <t>Av. Salaverry 300</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Av. Salverry 300, Candarave, Tacna, Tacna, Perú</t>
+          <t>Av. Salaverry 300, Candarave, Tacna, Tacna, Perú</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>-18.028091</v>
+        <v>-12.097018</v>
       </c>
       <c r="G6" t="n">
-        <v>-70.27267500000001</v>
+        <v>-77.055646</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Oficina Sur</t>
+          <t>Oficina Centro</t>
         </is>
       </c>
     </row>

</xml_diff>